<commit_message>
update VGP database files
</commit_message>
<xml_diff>
--- a/data/vgp_database/Bighorn_Basin_sediments.xlsx
+++ b/data/vgp_database/Bighorn_Basin_sediments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="166">
   <si>
     <t>Name:</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>mudstone; siltsone; sandstone</t>
-  </si>
-  <si>
-    <t>K?</t>
   </si>
   <si>
     <t>Clyde et al. (2007)</t>
@@ -578,7 +575,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -589,12 +586,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -666,12 +657,12 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1264,8 +1255,8 @@
       <c r="AA5" s="12">
         <v>1.0</v>
       </c>
-      <c r="AB5" s="18" t="s">
-        <v>46</v>
+      <c r="AB5" s="18">
+        <v>1.0</v>
       </c>
       <c r="AC5" s="12">
         <v>1.0</v>
@@ -1286,13 +1277,13 @@
         <v>1.0</v>
       </c>
       <c r="AI5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ5" s="19" t="s">
+      <c r="AK5" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="AK5" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="AL5" s="21"/>
     </row>
@@ -1341,7 +1332,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1390,7 +1381,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>5</v>
@@ -1399,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>8</v>
@@ -1417,10 +1408,10 @@
         <v>12</v>
       </c>
       <c r="K8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>15</v>
@@ -1462,31 +1453,31 @@
         <v>27</v>
       </c>
       <c r="Z8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AA8" s="8" t="s">
+      <c r="AB8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AB8" s="3" t="s">
+      <c r="AC8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AD8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AD8" s="3" t="s">
+      <c r="AE8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AE8" s="3" t="s">
+      <c r="AF8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AF8" s="3" t="s">
+      <c r="AG8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AG8" s="3" t="s">
+      <c r="AH8" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="AH8" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="AI8" s="3" t="s">
         <v>37</v>
@@ -1508,10 +1499,10 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>65</v>
       </c>
       <c r="C9" s="25">
         <v>44.69721</v>
@@ -1569,7 +1560,7 @@
         <v>45</v>
       </c>
       <c r="Z9" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA9" s="24">
         <v>1.0</v>
@@ -1578,7 +1569,7 @@
         <v>0.0</v>
       </c>
       <c r="AC9" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD9" s="24">
         <v>1.0</v>
@@ -1596,14 +1587,14 @@
         <v>4.0</v>
       </c>
       <c r="AI9" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ9" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ9" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK9" s="29"/>
       <c r="AL9" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM9" s="6"/>
       <c r="AN9" s="6"/>
@@ -1612,10 +1603,10 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="25">
         <v>44.69736</v>
@@ -1673,7 +1664,7 @@
         <v>45</v>
       </c>
       <c r="Z10" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA10" s="24">
         <v>1.0</v>
@@ -1682,7 +1673,7 @@
         <v>0.0</v>
       </c>
       <c r="AC10" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD10" s="24">
         <v>1.0</v>
@@ -1698,14 +1689,14 @@
       </c>
       <c r="AH10" s="21"/>
       <c r="AI10" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ10" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ10" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK10" s="29"/>
       <c r="AL10" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM10" s="6"/>
       <c r="AN10" s="6"/>
@@ -1714,10 +1705,10 @@
     </row>
     <row r="11">
       <c r="A11" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="25">
         <v>44.69695</v>
@@ -1775,7 +1766,7 @@
         <v>45</v>
       </c>
       <c r="Z11" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA11" s="24">
         <v>1.0</v>
@@ -1800,14 +1791,14 @@
       </c>
       <c r="AH11" s="21"/>
       <c r="AI11" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ11" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ11" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK11" s="29"/>
       <c r="AL11" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
@@ -1816,10 +1807,10 @@
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="25">
         <v>44.69677</v>
@@ -1877,7 +1868,7 @@
         <v>45</v>
       </c>
       <c r="Z12" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA12" s="24">
         <v>1.0</v>
@@ -1902,14 +1893,14 @@
       </c>
       <c r="AH12" s="21"/>
       <c r="AI12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ12" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ12" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK12" s="29"/>
       <c r="AL12" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM12" s="6"/>
       <c r="AN12" s="6"/>
@@ -1918,10 +1909,10 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="25">
         <v>44.69627</v>
@@ -1979,7 +1970,7 @@
         <v>45</v>
       </c>
       <c r="Z13" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA13" s="24">
         <v>1.0</v>
@@ -2004,14 +1995,14 @@
       </c>
       <c r="AH13" s="21"/>
       <c r="AI13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ13" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ13" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK13" s="29"/>
       <c r="AL13" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM13" s="6"/>
       <c r="AN13" s="6"/>
@@ -2020,10 +2011,10 @@
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="25">
         <v>44.69558</v>
@@ -2081,7 +2072,7 @@
         <v>45</v>
       </c>
       <c r="Z14" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA14" s="24">
         <v>1.0</v>
@@ -2106,14 +2097,14 @@
       </c>
       <c r="AH14" s="21"/>
       <c r="AI14" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ14" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ14" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK14" s="29"/>
       <c r="AL14" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM14" s="6"/>
       <c r="AN14" s="6"/>
@@ -2122,10 +2113,10 @@
     </row>
     <row r="15">
       <c r="A15" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="25">
         <v>44.69559</v>
@@ -2183,7 +2174,7 @@
         <v>45</v>
       </c>
       <c r="Z15" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA15" s="24">
         <v>1.0</v>
@@ -2208,14 +2199,14 @@
       </c>
       <c r="AH15" s="21"/>
       <c r="AI15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ15" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ15" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK15" s="29"/>
       <c r="AL15" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM15" s="6"/>
       <c r="AN15" s="6"/>
@@ -2224,10 +2215,10 @@
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="25">
         <v>44.69464</v>
@@ -2285,7 +2276,7 @@
         <v>45</v>
       </c>
       <c r="Z16" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA16" s="24">
         <v>1.0</v>
@@ -2310,14 +2301,14 @@
       </c>
       <c r="AH16" s="21"/>
       <c r="AI16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ16" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ16" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK16" s="29"/>
       <c r="AL16" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM16" s="6"/>
       <c r="AN16" s="6"/>
@@ -2326,10 +2317,10 @@
     </row>
     <row r="17">
       <c r="A17" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="25">
         <v>44.6939</v>
@@ -2387,7 +2378,7 @@
         <v>45</v>
       </c>
       <c r="Z17" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA17" s="24">
         <v>1.0</v>
@@ -2396,7 +2387,7 @@
         <v>0.0</v>
       </c>
       <c r="AC17" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD17" s="24">
         <v>1.0</v>
@@ -2414,16 +2405,16 @@
         <v>4.0</v>
       </c>
       <c r="AI17" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ17" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK17" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL17" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM17" s="6"/>
       <c r="AN17" s="6"/>
@@ -2432,10 +2423,10 @@
     </row>
     <row r="18">
       <c r="A18" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="25">
         <v>44.69375</v>
@@ -2493,7 +2484,7 @@
         <v>45</v>
       </c>
       <c r="Z18" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA18" s="24">
         <v>1.0</v>
@@ -2502,7 +2493,7 @@
         <v>0.0</v>
       </c>
       <c r="AC18" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD18" s="24">
         <v>1.0</v>
@@ -2518,14 +2509,14 @@
       </c>
       <c r="AH18" s="21"/>
       <c r="AI18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ18" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ18" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK18" s="29"/>
       <c r="AL18" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM18" s="6"/>
       <c r="AN18" s="6"/>
@@ -2534,10 +2525,10 @@
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="25">
         <v>44.69342</v>
@@ -2595,7 +2586,7 @@
         <v>45</v>
       </c>
       <c r="Z19" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA19" s="24">
         <v>1.0</v>
@@ -2604,7 +2595,7 @@
         <v>0.0</v>
       </c>
       <c r="AC19" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD19" s="24">
         <v>1.0</v>
@@ -2622,16 +2613,16 @@
         <v>4.0</v>
       </c>
       <c r="AI19" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ19" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ19" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK19" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL19" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM19" s="6"/>
       <c r="AN19" s="6"/>
@@ -2640,10 +2631,10 @@
     </row>
     <row r="20">
       <c r="A20" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="25">
         <v>44.69043</v>
@@ -2701,7 +2692,7 @@
         <v>45</v>
       </c>
       <c r="Z20" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA20" s="24">
         <v>1.0</v>
@@ -2710,7 +2701,7 @@
         <v>0.0</v>
       </c>
       <c r="AC20" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD20" s="24">
         <v>1.0</v>
@@ -2728,16 +2719,16 @@
         <v>4.0</v>
       </c>
       <c r="AI20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ20" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK20" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL20" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM20" s="6"/>
       <c r="AN20" s="6"/>
@@ -2746,10 +2737,10 @@
     </row>
     <row r="21">
       <c r="A21" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="25">
         <v>44.69029</v>
@@ -2807,7 +2798,7 @@
         <v>45</v>
       </c>
       <c r="Z21" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA21" s="24">
         <v>1.0</v>
@@ -2816,7 +2807,7 @@
         <v>0.0</v>
       </c>
       <c r="AC21" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD21" s="24">
         <v>1.0</v>
@@ -2834,16 +2825,16 @@
         <v>4.0</v>
       </c>
       <c r="AI21" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ21" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ21" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK21" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL21" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM21" s="6"/>
       <c r="AN21" s="6"/>
@@ -2852,10 +2843,10 @@
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="25">
         <v>44.68957</v>
@@ -2913,7 +2904,7 @@
         <v>45</v>
       </c>
       <c r="Z22" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA22" s="24">
         <v>1.0</v>
@@ -2922,7 +2913,7 @@
         <v>0.0</v>
       </c>
       <c r="AC22" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD22" s="24">
         <v>1.0</v>
@@ -2940,16 +2931,16 @@
         <v>4.0</v>
       </c>
       <c r="AI22" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ22" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ22" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK22" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL22" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM22" s="6"/>
       <c r="AN22" s="6"/>
@@ -2958,10 +2949,10 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="25">
         <v>44.68953</v>
@@ -3019,7 +3010,7 @@
         <v>45</v>
       </c>
       <c r="Z23" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA23" s="24">
         <v>1.0</v>
@@ -3028,7 +3019,7 @@
         <v>0.0</v>
       </c>
       <c r="AC23" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD23" s="24">
         <v>1.0</v>
@@ -3046,16 +3037,16 @@
         <v>4.0</v>
       </c>
       <c r="AI23" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ23" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ23" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK23" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL23" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM23" s="6"/>
       <c r="AN23" s="6"/>
@@ -3064,10 +3055,10 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="25">
         <v>44.68957</v>
@@ -3125,7 +3116,7 @@
         <v>45</v>
       </c>
       <c r="Z24" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA24" s="24">
         <v>1.0</v>
@@ -3134,7 +3125,7 @@
         <v>0.0</v>
       </c>
       <c r="AC24" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD24" s="24">
         <v>1.0</v>
@@ -3150,14 +3141,14 @@
       </c>
       <c r="AH24" s="21"/>
       <c r="AI24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ24" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ24" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK24" s="29"/>
       <c r="AL24" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM24" s="6"/>
       <c r="AN24" s="6"/>
@@ -3166,10 +3157,10 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="25">
         <v>44.68882</v>
@@ -3227,7 +3218,7 @@
         <v>45</v>
       </c>
       <c r="Z25" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA25" s="24">
         <v>1.0</v>
@@ -3252,14 +3243,14 @@
       </c>
       <c r="AH25" s="21"/>
       <c r="AI25" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ25" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ25" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK25" s="29"/>
       <c r="AL25" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM25" s="6"/>
       <c r="AN25" s="6"/>
@@ -3268,10 +3259,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="25">
         <v>44.68832</v>
@@ -3329,7 +3320,7 @@
         <v>45</v>
       </c>
       <c r="Z26" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA26" s="24">
         <v>1.0</v>
@@ -3338,7 +3329,7 @@
         <v>0.0</v>
       </c>
       <c r="AC26" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD26" s="24">
         <v>1.0</v>
@@ -3354,14 +3345,14 @@
       </c>
       <c r="AH26" s="21"/>
       <c r="AI26" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ26" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ26" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK26" s="29"/>
       <c r="AL26" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM26" s="6"/>
       <c r="AN26" s="6"/>
@@ -3370,10 +3361,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="25">
         <v>44.68824</v>
@@ -3431,7 +3422,7 @@
         <v>45</v>
       </c>
       <c r="Z27" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA27" s="24">
         <v>1.0</v>
@@ -3440,7 +3431,7 @@
         <v>0.0</v>
       </c>
       <c r="AC27" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD27" s="24">
         <v>1.0</v>
@@ -3458,16 +3449,16 @@
         <v>4.0</v>
       </c>
       <c r="AI27" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ27" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ27" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK27" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL27" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM27" s="6"/>
       <c r="AN27" s="6"/>
@@ -3476,10 +3467,10 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="25">
         <v>44.68565</v>
@@ -3537,7 +3528,7 @@
         <v>45</v>
       </c>
       <c r="Z28" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA28" s="24">
         <v>1.0</v>
@@ -3562,14 +3553,14 @@
       </c>
       <c r="AH28" s="21"/>
       <c r="AI28" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ28" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ28" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK28" s="29"/>
       <c r="AL28" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM28" s="6"/>
       <c r="AN28" s="6"/>
@@ -3578,10 +3569,10 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="25">
         <v>44.6843</v>
@@ -3639,7 +3630,7 @@
         <v>45</v>
       </c>
       <c r="Z29" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA29" s="24">
         <v>1.0</v>
@@ -3664,14 +3655,14 @@
       </c>
       <c r="AH29" s="21"/>
       <c r="AI29" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ29" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ29" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK29" s="29"/>
       <c r="AL29" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM29" s="6"/>
       <c r="AN29" s="6"/>
@@ -3680,10 +3671,10 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="25">
         <v>44.68416</v>
@@ -3741,7 +3732,7 @@
         <v>45</v>
       </c>
       <c r="Z30" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA30" s="24">
         <v>1.0</v>
@@ -3766,14 +3757,14 @@
       </c>
       <c r="AH30" s="21"/>
       <c r="AI30" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ30" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ30" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK30" s="29"/>
       <c r="AL30" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM30" s="6"/>
       <c r="AN30" s="6"/>
@@ -3782,10 +3773,10 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="25">
         <v>44.68322</v>
@@ -3843,7 +3834,7 @@
         <v>45</v>
       </c>
       <c r="Z31" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA31" s="24">
         <v>1.0</v>
@@ -3868,14 +3859,14 @@
       </c>
       <c r="AH31" s="21"/>
       <c r="AI31" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ31" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ31" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK31" s="29"/>
       <c r="AL31" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM31" s="6"/>
       <c r="AN31" s="6"/>
@@ -3884,10 +3875,10 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="25">
         <v>44.6797</v>
@@ -3945,7 +3936,7 @@
         <v>45</v>
       </c>
       <c r="Z32" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA32" s="24">
         <v>1.0</v>
@@ -3970,14 +3961,14 @@
       </c>
       <c r="AH32" s="21"/>
       <c r="AI32" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ32" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ32" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK32" s="29"/>
       <c r="AL32" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM32" s="6"/>
       <c r="AN32" s="6"/>
@@ -3986,10 +3977,10 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="25">
         <v>44.67902</v>
@@ -4047,7 +4038,7 @@
         <v>45</v>
       </c>
       <c r="Z33" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA33" s="24">
         <v>1.0</v>
@@ -4072,14 +4063,14 @@
       </c>
       <c r="AH33" s="21"/>
       <c r="AI33" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ33" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ33" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK33" s="29"/>
       <c r="AL33" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM33" s="6"/>
       <c r="AN33" s="6"/>
@@ -4088,10 +4079,10 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="25">
         <v>44.6784</v>
@@ -4149,7 +4140,7 @@
         <v>45</v>
       </c>
       <c r="Z34" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA34" s="24">
         <v>1.0</v>
@@ -4174,14 +4165,14 @@
       </c>
       <c r="AH34" s="21"/>
       <c r="AI34" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ34" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ34" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK34" s="29"/>
       <c r="AL34" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM34" s="6"/>
       <c r="AN34" s="6"/>
@@ -4190,10 +4181,10 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="25">
         <v>44.67852</v>
@@ -4251,7 +4242,7 @@
         <v>45</v>
       </c>
       <c r="Z35" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA35" s="24">
         <v>1.0</v>
@@ -4276,14 +4267,14 @@
       </c>
       <c r="AH35" s="21"/>
       <c r="AI35" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ35" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ35" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK35" s="29"/>
       <c r="AL35" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM35" s="6"/>
       <c r="AN35" s="6"/>
@@ -4292,10 +4283,10 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="25">
         <v>44.67783</v>
@@ -4353,7 +4344,7 @@
         <v>45</v>
       </c>
       <c r="Z36" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA36" s="24">
         <v>1.0</v>
@@ -4378,14 +4369,14 @@
       </c>
       <c r="AH36" s="21"/>
       <c r="AI36" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ36" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ36" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK36" s="29"/>
       <c r="AL36" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM36" s="6"/>
       <c r="AN36" s="6"/>
@@ -4394,10 +4385,10 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" s="25">
         <v>44.67775</v>
@@ -4455,7 +4446,7 @@
         <v>45</v>
       </c>
       <c r="Z37" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA37" s="24">
         <v>1.0</v>
@@ -4480,14 +4471,14 @@
       </c>
       <c r="AH37" s="21"/>
       <c r="AI37" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ37" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ37" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK37" s="29"/>
       <c r="AL37" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM37" s="6"/>
       <c r="AN37" s="6"/>
@@ -4496,10 +4487,10 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="25">
         <v>44.67763</v>
@@ -4557,7 +4548,7 @@
         <v>45</v>
       </c>
       <c r="Z38" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA38" s="24">
         <v>1.0</v>
@@ -4582,14 +4573,14 @@
       </c>
       <c r="AH38" s="21"/>
       <c r="AI38" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ38" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ38" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK38" s="29"/>
       <c r="AL38" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -4598,10 +4589,10 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="25">
         <v>44.67675</v>
@@ -4659,7 +4650,7 @@
         <v>45</v>
       </c>
       <c r="Z39" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA39" s="24">
         <v>1.0</v>
@@ -4684,14 +4675,14 @@
       </c>
       <c r="AH39" s="21"/>
       <c r="AI39" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ39" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ39" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK39" s="29"/>
       <c r="AL39" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM39" s="6"/>
       <c r="AN39" s="6"/>
@@ -4700,10 +4691,10 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="25">
         <v>44.67668</v>
@@ -4761,7 +4752,7 @@
         <v>45</v>
       </c>
       <c r="Z40" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA40" s="24">
         <v>1.0</v>
@@ -4786,14 +4777,14 @@
       </c>
       <c r="AH40" s="21"/>
       <c r="AI40" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ40" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ40" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK40" s="29"/>
       <c r="AL40" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM40" s="6"/>
       <c r="AN40" s="6"/>
@@ -4802,10 +4793,10 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="25">
         <v>44.67668</v>
@@ -4863,7 +4854,7 @@
         <v>45</v>
       </c>
       <c r="Z41" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA41" s="24">
         <v>1.0</v>
@@ -4888,14 +4879,14 @@
       </c>
       <c r="AH41" s="21"/>
       <c r="AI41" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ41" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ41" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK41" s="29"/>
       <c r="AL41" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM41" s="6"/>
       <c r="AN41" s="6"/>
@@ -4904,10 +4895,10 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" s="25">
         <v>44.67356</v>
@@ -4965,7 +4956,7 @@
         <v>45</v>
       </c>
       <c r="Z42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA42" s="24">
         <v>1.0</v>
@@ -4990,14 +4981,14 @@
       </c>
       <c r="AH42" s="21"/>
       <c r="AI42" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ42" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ42" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK42" s="29"/>
       <c r="AL42" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM42" s="6"/>
       <c r="AN42" s="6"/>
@@ -5006,10 +4997,10 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="25">
         <v>44.67377</v>
@@ -5067,7 +5058,7 @@
         <v>45</v>
       </c>
       <c r="Z43" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA43" s="24">
         <v>1.0</v>
@@ -5092,14 +5083,14 @@
       </c>
       <c r="AH43" s="21"/>
       <c r="AI43" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ43" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ43" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK43" s="29"/>
       <c r="AL43" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM43" s="6"/>
       <c r="AN43" s="6"/>
@@ -5108,10 +5099,10 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" s="25">
         <v>44.67128</v>
@@ -5169,7 +5160,7 @@
         <v>45</v>
       </c>
       <c r="Z44" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA44" s="24">
         <v>1.0</v>
@@ -5178,7 +5169,7 @@
         <v>0.0</v>
       </c>
       <c r="AC44" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD44" s="24">
         <v>2.0</v>
@@ -5194,14 +5185,14 @@
       </c>
       <c r="AH44" s="21"/>
       <c r="AI44" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ44" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ44" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK44" s="29"/>
       <c r="AL44" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM44" s="6"/>
       <c r="AN44" s="6"/>
@@ -5210,10 +5201,10 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="25">
         <v>44.67047</v>
@@ -5271,7 +5262,7 @@
         <v>45</v>
       </c>
       <c r="Z45" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA45" s="24">
         <v>1.0</v>
@@ -5280,7 +5271,7 @@
         <v>0.0</v>
       </c>
       <c r="AC45" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD45" s="24">
         <v>2.0</v>
@@ -5296,14 +5287,14 @@
       </c>
       <c r="AH45" s="21"/>
       <c r="AI45" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ45" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ45" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK45" s="29"/>
       <c r="AL45" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM45" s="6"/>
       <c r="AN45" s="6"/>
@@ -5312,10 +5303,10 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="25">
         <v>44.66419</v>
@@ -5373,7 +5364,7 @@
         <v>45</v>
       </c>
       <c r="Z46" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA46" s="24">
         <v>1.0</v>
@@ -5382,7 +5373,7 @@
         <v>0.0</v>
       </c>
       <c r="AC46" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD46" s="24">
         <v>2.0</v>
@@ -5400,16 +5391,16 @@
         <v>4.0</v>
       </c>
       <c r="AI46" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ46" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ46" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK46" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL46" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM46" s="6"/>
       <c r="AN46" s="6"/>
@@ -5418,10 +5409,10 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="25">
         <v>44.65185</v>
@@ -5479,7 +5470,7 @@
         <v>45</v>
       </c>
       <c r="Z47" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA47" s="24">
         <v>1.0</v>
@@ -5488,7 +5479,7 @@
         <v>0.0</v>
       </c>
       <c r="AC47" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD47" s="24">
         <v>2.0</v>
@@ -5506,16 +5497,16 @@
         <v>4.0</v>
       </c>
       <c r="AI47" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ47" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ47" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK47" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL47" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM47" s="6"/>
       <c r="AN47" s="6"/>
@@ -5524,10 +5515,10 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" s="25">
         <v>44.17225</v>
@@ -5585,7 +5576,7 @@
         <v>45</v>
       </c>
       <c r="Z48" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA48" s="24">
         <v>1.0</v>
@@ -5610,14 +5601,14 @@
       </c>
       <c r="AH48" s="21"/>
       <c r="AI48" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ48" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ48" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK48" s="29"/>
       <c r="AL48" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM48" s="6"/>
       <c r="AN48" s="6"/>
@@ -5626,10 +5617,10 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" s="25">
         <v>44.17173</v>
@@ -5687,7 +5678,7 @@
         <v>45</v>
       </c>
       <c r="Z49" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA49" s="24">
         <v>1.0</v>
@@ -5712,14 +5703,14 @@
       </c>
       <c r="AH49" s="21"/>
       <c r="AI49" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ49" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ49" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK49" s="29"/>
       <c r="AL49" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM49" s="6"/>
       <c r="AN49" s="6"/>
@@ -5728,10 +5719,10 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" s="25">
         <v>44.17166</v>
@@ -5789,7 +5780,7 @@
         <v>45</v>
       </c>
       <c r="Z50" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA50" s="24">
         <v>1.0</v>
@@ -5814,14 +5805,14 @@
       </c>
       <c r="AH50" s="21"/>
       <c r="AI50" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ50" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ50" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK50" s="29"/>
       <c r="AL50" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM50" s="6"/>
       <c r="AN50" s="6"/>
@@ -5830,10 +5821,10 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="25">
         <v>44.17063</v>
@@ -5891,7 +5882,7 @@
         <v>45</v>
       </c>
       <c r="Z51" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA51" s="24">
         <v>1.0</v>
@@ -5900,7 +5891,7 @@
         <v>0.0</v>
       </c>
       <c r="AC51" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD51" s="24">
         <v>3.0</v>
@@ -5916,14 +5907,14 @@
       </c>
       <c r="AH51" s="21"/>
       <c r="AI51" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ51" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ51" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK51" s="29"/>
       <c r="AL51" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM51" s="6"/>
       <c r="AN51" s="6"/>
@@ -5932,10 +5923,10 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="25">
         <v>44.17162</v>
@@ -5993,7 +5984,7 @@
         <v>45</v>
       </c>
       <c r="Z52" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA52" s="24">
         <v>1.0</v>
@@ -6002,7 +5993,7 @@
         <v>0.0</v>
       </c>
       <c r="AC52" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD52" s="24">
         <v>3.0</v>
@@ -6020,16 +6011,16 @@
         <v>4.0</v>
       </c>
       <c r="AI52" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ52" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ52" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK52" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL52" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM52" s="6"/>
       <c r="AN52" s="6"/>
@@ -6038,10 +6029,10 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="25">
         <v>44.17154</v>
@@ -6099,7 +6090,7 @@
         <v>45</v>
       </c>
       <c r="Z53" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA53" s="24">
         <v>1.0</v>
@@ -6108,7 +6099,7 @@
         <v>0.0</v>
       </c>
       <c r="AC53" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD53" s="24">
         <v>3.0</v>
@@ -6126,16 +6117,16 @@
         <v>4.0</v>
       </c>
       <c r="AI53" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ53" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ53" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK53" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL53" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM53" s="6"/>
       <c r="AN53" s="6"/>
@@ -6144,10 +6135,10 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" s="25">
         <v>44.17147</v>
@@ -6205,7 +6196,7 @@
         <v>45</v>
       </c>
       <c r="Z54" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA54" s="24">
         <v>1.0</v>
@@ -6214,7 +6205,7 @@
         <v>0.0</v>
       </c>
       <c r="AC54" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD54" s="24">
         <v>3.0</v>
@@ -6232,16 +6223,16 @@
         <v>4.0</v>
       </c>
       <c r="AI54" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ54" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ54" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK54" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL54" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM54" s="6"/>
       <c r="AN54" s="6"/>
@@ -6250,10 +6241,10 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="25">
         <v>44.17128</v>
@@ -6311,7 +6302,7 @@
         <v>45</v>
       </c>
       <c r="Z55" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA55" s="24">
         <v>1.0</v>
@@ -6320,7 +6311,7 @@
         <v>0.0</v>
       </c>
       <c r="AC55" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD55" s="24">
         <v>3.0</v>
@@ -6336,14 +6327,14 @@
       </c>
       <c r="AH55" s="21"/>
       <c r="AI55" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ55" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ55" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK55" s="29"/>
       <c r="AL55" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM55" s="6"/>
       <c r="AN55" s="6"/>
@@ -6352,10 +6343,10 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56" s="25">
         <v>44.17137</v>
@@ -6413,7 +6404,7 @@
         <v>45</v>
       </c>
       <c r="Z56" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA56" s="24">
         <v>1.0</v>
@@ -6438,14 +6429,14 @@
       </c>
       <c r="AH56" s="21"/>
       <c r="AI56" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ56" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ56" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK56" s="29"/>
       <c r="AL56" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM56" s="6"/>
       <c r="AN56" s="6"/>
@@ -6454,10 +6445,10 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="25">
         <v>44.17114</v>
@@ -6515,7 +6506,7 @@
         <v>45</v>
       </c>
       <c r="Z57" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA57" s="24">
         <v>1.0</v>
@@ -6524,7 +6515,7 @@
         <v>0.0</v>
       </c>
       <c r="AC57" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD57" s="24">
         <v>3.0</v>
@@ -6540,14 +6531,14 @@
       </c>
       <c r="AH57" s="21"/>
       <c r="AI57" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ57" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ57" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK57" s="29"/>
       <c r="AL57" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM57" s="6"/>
       <c r="AN57" s="6"/>
@@ -6556,10 +6547,10 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" s="25">
         <v>44.16997</v>
@@ -6617,7 +6608,7 @@
         <v>45</v>
       </c>
       <c r="Z58" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA58" s="24">
         <v>1.0</v>
@@ -6626,7 +6617,7 @@
         <v>0.0</v>
       </c>
       <c r="AC58" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD58" s="24">
         <v>3.0</v>
@@ -6644,16 +6635,16 @@
         <v>4.0</v>
       </c>
       <c r="AI58" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ58" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ58" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK58" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL58" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM58" s="6"/>
       <c r="AN58" s="6"/>
@@ -6662,10 +6653,10 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="25">
         <v>44.16987</v>
@@ -6723,7 +6714,7 @@
         <v>45</v>
       </c>
       <c r="Z59" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA59" s="24">
         <v>1.0</v>
@@ -6732,7 +6723,7 @@
         <v>0.0</v>
       </c>
       <c r="AC59" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD59" s="24">
         <v>3.0</v>
@@ -6750,16 +6741,16 @@
         <v>4.0</v>
       </c>
       <c r="AI59" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ59" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ59" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK59" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL59" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM59" s="6"/>
       <c r="AN59" s="6"/>
@@ -6768,10 +6759,10 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" s="25">
         <v>44.16962</v>
@@ -6829,7 +6820,7 @@
         <v>45</v>
       </c>
       <c r="Z60" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA60" s="24">
         <v>1.0</v>
@@ -6838,7 +6829,7 @@
         <v>0.0</v>
       </c>
       <c r="AC60" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD60" s="24">
         <v>3.0</v>
@@ -6854,14 +6845,14 @@
       </c>
       <c r="AH60" s="21"/>
       <c r="AI60" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ60" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ60" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK60" s="29"/>
       <c r="AL60" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM60" s="6"/>
       <c r="AN60" s="6"/>
@@ -6870,10 +6861,10 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="25">
         <v>44.1697</v>
@@ -6931,7 +6922,7 @@
         <v>45</v>
       </c>
       <c r="Z61" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA61" s="24">
         <v>1.0</v>
@@ -6940,7 +6931,7 @@
         <v>0.0</v>
       </c>
       <c r="AC61" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD61" s="24">
         <v>3.0</v>
@@ -6956,14 +6947,14 @@
       </c>
       <c r="AH61" s="21"/>
       <c r="AI61" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ61" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ61" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK61" s="29"/>
       <c r="AL61" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM61" s="6"/>
       <c r="AN61" s="6"/>
@@ -6972,10 +6963,10 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C62" s="25">
         <v>44.1696</v>
@@ -7033,7 +7024,7 @@
         <v>45</v>
       </c>
       <c r="Z62" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA62" s="24">
         <v>1.0</v>
@@ -7042,7 +7033,7 @@
         <v>0.0</v>
       </c>
       <c r="AC62" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD62" s="24">
         <v>3.0</v>
@@ -7058,14 +7049,14 @@
       </c>
       <c r="AH62" s="21"/>
       <c r="AI62" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ62" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ62" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK62" s="29"/>
       <c r="AL62" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM62" s="6"/>
       <c r="AN62" s="6"/>
@@ -7074,10 +7065,10 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63" s="25">
         <v>44.16765</v>
@@ -7135,7 +7126,7 @@
         <v>45</v>
       </c>
       <c r="Z63" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA63" s="24">
         <v>1.0</v>
@@ -7160,14 +7151,14 @@
       </c>
       <c r="AH63" s="21"/>
       <c r="AI63" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ63" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ63" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK63" s="29"/>
       <c r="AL63" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM63" s="6"/>
       <c r="AN63" s="6"/>
@@ -7176,10 +7167,10 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" s="25">
         <v>44.16728</v>
@@ -7237,7 +7228,7 @@
         <v>45</v>
       </c>
       <c r="Z64" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA64" s="24">
         <v>1.0</v>
@@ -7262,14 +7253,14 @@
       </c>
       <c r="AH64" s="21"/>
       <c r="AI64" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ64" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ64" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK64" s="29"/>
       <c r="AL64" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM64" s="6"/>
       <c r="AN64" s="6"/>
@@ -7278,10 +7269,10 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="25">
         <v>44.16663</v>
@@ -7339,7 +7330,7 @@
         <v>45</v>
       </c>
       <c r="Z65" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA65" s="24">
         <v>1.0</v>
@@ -7364,14 +7355,14 @@
       </c>
       <c r="AH65" s="21"/>
       <c r="AI65" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ65" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ65" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK65" s="29"/>
       <c r="AL65" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM65" s="6"/>
       <c r="AN65" s="6"/>
@@ -7380,10 +7371,10 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C66" s="25">
         <v>44.16593</v>
@@ -7441,7 +7432,7 @@
         <v>45</v>
       </c>
       <c r="Z66" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA66" s="24">
         <v>1.0</v>
@@ -7468,16 +7459,16 @@
         <v>4.0</v>
       </c>
       <c r="AI66" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ66" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ66" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK66" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL66" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM66" s="6"/>
       <c r="AN66" s="6"/>
@@ -7486,10 +7477,10 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="25">
         <v>44.16568</v>
@@ -7547,7 +7538,7 @@
         <v>45</v>
       </c>
       <c r="Z67" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA67" s="24">
         <v>1.0</v>
@@ -7572,14 +7563,14 @@
       </c>
       <c r="AH67" s="21"/>
       <c r="AI67" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ67" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ67" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK67" s="29"/>
       <c r="AL67" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM67" s="6"/>
       <c r="AN67" s="6"/>
@@ -7588,10 +7579,10 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C68" s="25">
         <v>44.16576</v>
@@ -7649,7 +7640,7 @@
         <v>45</v>
       </c>
       <c r="Z68" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA68" s="24">
         <v>1.0</v>
@@ -7676,16 +7667,16 @@
         <v>4.0</v>
       </c>
       <c r="AI68" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ68" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ68" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK68" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL68" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM68" s="6"/>
       <c r="AN68" s="6"/>
@@ -7694,10 +7685,10 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" s="25">
         <v>44.16787</v>
@@ -7755,7 +7746,7 @@
         <v>45</v>
       </c>
       <c r="Z69" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA69" s="24">
         <v>1.0</v>
@@ -7764,7 +7755,7 @@
         <v>0.0</v>
       </c>
       <c r="AC69" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD69" s="24">
         <v>3.0</v>
@@ -7780,14 +7771,14 @@
       </c>
       <c r="AH69" s="21"/>
       <c r="AI69" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ69" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ69" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK69" s="29"/>
       <c r="AL69" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM69" s="6"/>
       <c r="AN69" s="6"/>
@@ -7796,10 +7787,10 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C70" s="25">
         <v>44.1672</v>
@@ -7857,7 +7848,7 @@
         <v>45</v>
       </c>
       <c r="Z70" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA70" s="24">
         <v>1.0</v>
@@ -7866,7 +7857,7 @@
         <v>0.0</v>
       </c>
       <c r="AC70" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD70" s="24">
         <v>3.0</v>
@@ -7884,16 +7875,16 @@
         <v>4.0</v>
       </c>
       <c r="AI70" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ70" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ70" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK70" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL70" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM70" s="6"/>
       <c r="AN70" s="6"/>
@@ -7902,10 +7893,10 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C71" s="25">
         <v>44.16707</v>
@@ -7963,7 +7954,7 @@
         <v>45</v>
       </c>
       <c r="Z71" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA71" s="24">
         <v>1.0</v>
@@ -7972,7 +7963,7 @@
         <v>0.0</v>
       </c>
       <c r="AC71" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD71" s="24">
         <v>3.0</v>
@@ -7990,16 +7981,16 @@
         <v>4.0</v>
       </c>
       <c r="AI71" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ71" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ71" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK71" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL71" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM71" s="6"/>
       <c r="AN71" s="6"/>
@@ -8008,10 +7999,10 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C72" s="25">
         <v>44.16426</v>
@@ -8069,7 +8060,7 @@
         <v>45</v>
       </c>
       <c r="Z72" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA72" s="24">
         <v>1.0</v>
@@ -8078,7 +8069,7 @@
         <v>0.0</v>
       </c>
       <c r="AC72" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD72" s="24">
         <v>3.0</v>
@@ -8096,16 +8087,16 @@
         <v>4.0</v>
       </c>
       <c r="AI72" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ72" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ72" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK72" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL72" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM72" s="6"/>
       <c r="AN72" s="6"/>
@@ -8114,10 +8105,10 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="24" t="s">
         <v>135</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>136</v>
       </c>
       <c r="C73" s="25">
         <v>44.35619</v>
@@ -8175,7 +8166,7 @@
         <v>45</v>
       </c>
       <c r="Z73" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA73" s="24">
         <v>1.0</v>
@@ -8184,7 +8175,7 @@
         <v>0.0</v>
       </c>
       <c r="AC73" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD73" s="24">
         <v>4.0</v>
@@ -8200,14 +8191,14 @@
       </c>
       <c r="AH73" s="21"/>
       <c r="AI73" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ73" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ73" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK73" s="29"/>
       <c r="AL73" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM73" s="6"/>
       <c r="AN73" s="6"/>
@@ -8216,10 +8207,10 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C74" s="25">
         <v>44.35126</v>
@@ -8277,7 +8268,7 @@
         <v>45</v>
       </c>
       <c r="Z74" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA74" s="24">
         <v>1.0</v>
@@ -8286,7 +8277,7 @@
         <v>0.0</v>
       </c>
       <c r="AC74" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD74" s="24">
         <v>4.0</v>
@@ -8304,16 +8295,16 @@
         <v>4.0</v>
       </c>
       <c r="AI74" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ74" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ74" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK74" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL74" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM74" s="6"/>
       <c r="AN74" s="6"/>
@@ -8322,10 +8313,10 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C75" s="25">
         <v>44.34382</v>
@@ -8383,7 +8374,7 @@
         <v>45</v>
       </c>
       <c r="Z75" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA75" s="24">
         <v>1.0</v>
@@ -8392,7 +8383,7 @@
         <v>0.0</v>
       </c>
       <c r="AC75" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD75" s="24">
         <v>4.0</v>
@@ -8410,16 +8401,16 @@
         <v>4.0</v>
       </c>
       <c r="AI75" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ75" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ75" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK75" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL75" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM75" s="6"/>
       <c r="AN75" s="6"/>
@@ -8428,10 +8419,10 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C76" s="25">
         <v>44.30779</v>
@@ -8489,7 +8480,7 @@
         <v>45</v>
       </c>
       <c r="Z76" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA76" s="24">
         <v>1.0</v>
@@ -8498,7 +8489,7 @@
         <v>0.0</v>
       </c>
       <c r="AC76" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD76" s="24">
         <v>4.0</v>
@@ -8516,16 +8507,16 @@
         <v>4.0</v>
       </c>
       <c r="AI76" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ76" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ76" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK76" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL76" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM76" s="6"/>
       <c r="AN76" s="6"/>
@@ -8534,10 +8525,10 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C77" s="25">
         <v>44.30817</v>
@@ -8595,7 +8586,7 @@
         <v>45</v>
       </c>
       <c r="Z77" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA77" s="24">
         <v>1.0</v>
@@ -8604,7 +8595,7 @@
         <v>0.0</v>
       </c>
       <c r="AC77" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD77" s="24">
         <v>4.0</v>
@@ -8620,14 +8611,14 @@
       </c>
       <c r="AH77" s="21"/>
       <c r="AI77" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ77" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ77" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK77" s="29"/>
       <c r="AL77" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM77" s="6"/>
       <c r="AN77" s="6"/>
@@ -8636,10 +8627,10 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C78" s="25">
         <v>44.3332</v>
@@ -8697,7 +8688,7 @@
         <v>45</v>
       </c>
       <c r="Z78" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA78" s="24">
         <v>1.0</v>
@@ -8706,7 +8697,7 @@
         <v>0.0</v>
       </c>
       <c r="AC78" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD78" s="24">
         <v>4.0</v>
@@ -8724,16 +8715,16 @@
         <v>4.0</v>
       </c>
       <c r="AI78" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ78" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ78" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK78" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL78" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM78" s="6"/>
       <c r="AN78" s="6"/>
@@ -8742,10 +8733,10 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C79" s="25">
         <v>44.34137</v>
@@ -8803,7 +8794,7 @@
         <v>45</v>
       </c>
       <c r="Z79" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA79" s="24">
         <v>1.0</v>
@@ -8828,14 +8819,14 @@
       </c>
       <c r="AH79" s="21"/>
       <c r="AI79" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ79" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ79" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK79" s="29"/>
       <c r="AL79" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM79" s="6"/>
       <c r="AN79" s="6"/>
@@ -8844,10 +8835,10 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C80" s="25">
         <v>44.36538</v>
@@ -8905,7 +8896,7 @@
         <v>45</v>
       </c>
       <c r="Z80" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA80" s="24">
         <v>1.0</v>
@@ -8914,7 +8905,7 @@
         <v>0.0</v>
       </c>
       <c r="AC80" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD80" s="24">
         <v>5.0</v>
@@ -8930,14 +8921,14 @@
       </c>
       <c r="AH80" s="21"/>
       <c r="AI80" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ80" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ80" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK80" s="29"/>
       <c r="AL80" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM80" s="6"/>
       <c r="AN80" s="6"/>
@@ -8946,10 +8937,10 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C81" s="25">
         <v>44.3637</v>
@@ -9007,7 +8998,7 @@
         <v>45</v>
       </c>
       <c r="Z81" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA81" s="24">
         <v>1.0</v>
@@ -9016,7 +9007,7 @@
         <v>0.0</v>
       </c>
       <c r="AC81" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD81" s="24">
         <v>5.0</v>
@@ -9034,16 +9025,16 @@
         <v>4.0</v>
       </c>
       <c r="AI81" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ81" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ81" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK81" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL81" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM81" s="6"/>
       <c r="AN81" s="6"/>
@@ -9052,10 +9043,10 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C82" s="25">
         <v>44.36063</v>
@@ -9113,7 +9104,7 @@
         <v>45</v>
       </c>
       <c r="Z82" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA82" s="24">
         <v>1.0</v>
@@ -9138,14 +9129,14 @@
       </c>
       <c r="AH82" s="21"/>
       <c r="AI82" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ82" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ82" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK82" s="29"/>
       <c r="AL82" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM82" s="6"/>
       <c r="AN82" s="6"/>
@@ -9154,10 +9145,10 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C83" s="25">
         <v>44.3603</v>
@@ -9215,7 +9206,7 @@
         <v>45</v>
       </c>
       <c r="Z83" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA83" s="24">
         <v>1.0</v>
@@ -9224,7 +9215,7 @@
         <v>0.0</v>
       </c>
       <c r="AC83" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD83" s="24">
         <v>5.0</v>
@@ -9242,16 +9233,16 @@
         <v>4.0</v>
       </c>
       <c r="AI83" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ83" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ83" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK83" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL83" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM83" s="6"/>
       <c r="AN83" s="6"/>
@@ -9260,10 +9251,10 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C84" s="25">
         <v>44.35673</v>
@@ -9321,7 +9312,7 @@
         <v>45</v>
       </c>
       <c r="Z84" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA84" s="24">
         <v>1.0</v>
@@ -9330,7 +9321,7 @@
         <v>0.0</v>
       </c>
       <c r="AC84" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD84" s="24">
         <v>5.0</v>
@@ -9348,16 +9339,16 @@
         <v>4.0</v>
       </c>
       <c r="AI84" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ84" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ84" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK84" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL84" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM84" s="6"/>
       <c r="AN84" s="6"/>
@@ -9366,10 +9357,10 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C85" s="25">
         <v>44.35258</v>
@@ -9427,7 +9418,7 @@
         <v>45</v>
       </c>
       <c r="Z85" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA85" s="24">
         <v>1.0</v>
@@ -9436,7 +9427,7 @@
         <v>0.0</v>
       </c>
       <c r="AC85" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD85" s="24">
         <v>5.0</v>
@@ -9454,16 +9445,16 @@
         <v>4.0</v>
       </c>
       <c r="AI85" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ85" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ85" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK85" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL85" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM85" s="6"/>
       <c r="AN85" s="6"/>
@@ -9472,10 +9463,10 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" s="25">
         <v>44.35062</v>
@@ -9533,7 +9524,7 @@
         <v>45</v>
       </c>
       <c r="Z86" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA86" s="24">
         <v>1.0</v>
@@ -9542,7 +9533,7 @@
         <v>0.0</v>
       </c>
       <c r="AC86" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD86" s="24">
         <v>5.0</v>
@@ -9560,16 +9551,16 @@
         <v>4.0</v>
       </c>
       <c r="AI86" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ86" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ86" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK86" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL86" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM86" s="6"/>
       <c r="AN86" s="6"/>
@@ -9578,10 +9569,10 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C87" s="25">
         <v>44.33802</v>
@@ -9639,7 +9630,7 @@
         <v>45</v>
       </c>
       <c r="Z87" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA87" s="24">
         <v>1.0</v>
@@ -9648,7 +9639,7 @@
         <v>0.0</v>
       </c>
       <c r="AC87" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD87" s="24">
         <v>5.0</v>
@@ -9664,14 +9655,14 @@
       </c>
       <c r="AH87" s="21"/>
       <c r="AI87" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ87" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ87" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK87" s="29"/>
       <c r="AL87" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM87" s="6"/>
       <c r="AN87" s="6"/>
@@ -9680,10 +9671,10 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C88" s="25">
         <v>44.33749</v>
@@ -9741,7 +9732,7 @@
         <v>45</v>
       </c>
       <c r="Z88" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA88" s="24">
         <v>1.0</v>
@@ -9766,14 +9757,14 @@
       </c>
       <c r="AH88" s="21"/>
       <c r="AI88" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ88" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ88" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK88" s="29"/>
       <c r="AL88" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM88" s="6"/>
       <c r="AN88" s="6"/>
@@ -9782,10 +9773,10 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C89" s="25">
         <v>44.33812</v>
@@ -9843,7 +9834,7 @@
         <v>45</v>
       </c>
       <c r="Z89" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA89" s="24">
         <v>1.0</v>
@@ -9852,7 +9843,7 @@
         <v>0.0</v>
       </c>
       <c r="AC89" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD89" s="24">
         <v>5.0</v>
@@ -9870,16 +9861,16 @@
         <v>4.0</v>
       </c>
       <c r="AI89" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ89" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ89" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK89" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL89" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM89" s="6"/>
       <c r="AN89" s="6"/>
@@ -9888,10 +9879,10 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C90" s="25">
         <v>44.33149</v>
@@ -9949,7 +9940,7 @@
         <v>45</v>
       </c>
       <c r="Z90" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA90" s="24">
         <v>1.0</v>
@@ -9958,7 +9949,7 @@
         <v>0.0</v>
       </c>
       <c r="AC90" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD90" s="24">
         <v>5.0</v>
@@ -9976,16 +9967,16 @@
         <v>4.0</v>
       </c>
       <c r="AI90" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ90" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ90" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK90" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL90" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM90" s="6"/>
       <c r="AN90" s="6"/>
@@ -9994,10 +9985,10 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B91" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C91" s="25">
         <v>44.331</v>
@@ -10055,7 +10046,7 @@
         <v>45</v>
       </c>
       <c r="Z91" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA91" s="24">
         <v>1.0</v>
@@ -10064,7 +10055,7 @@
         <v>0.0</v>
       </c>
       <c r="AC91" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD91" s="24">
         <v>5.0</v>
@@ -10082,16 +10073,16 @@
         <v>4.0</v>
       </c>
       <c r="AI91" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ91" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ91" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK91" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL91" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM91" s="6"/>
       <c r="AN91" s="6"/>
@@ -10100,10 +10091,10 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B92" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C92" s="25">
         <v>44.331</v>
@@ -10161,7 +10152,7 @@
         <v>45</v>
       </c>
       <c r="Z92" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA92" s="24">
         <v>1.0</v>
@@ -10170,7 +10161,7 @@
         <v>0.0</v>
       </c>
       <c r="AC92" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD92" s="24">
         <v>5.0</v>
@@ -10188,16 +10179,16 @@
         <v>4.0</v>
       </c>
       <c r="AI92" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ92" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ92" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK92" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL92" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM92" s="6"/>
       <c r="AN92" s="6"/>
@@ -10206,10 +10197,10 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C93" s="25">
         <v>44.33</v>
@@ -10267,7 +10258,7 @@
         <v>45</v>
       </c>
       <c r="Z93" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA93" s="24">
         <v>1.0</v>
@@ -10292,14 +10283,14 @@
       </c>
       <c r="AH93" s="21"/>
       <c r="AI93" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ93" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ93" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK93" s="29"/>
       <c r="AL93" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM93" s="6"/>
       <c r="AN93" s="6"/>
@@ -10308,10 +10299,10 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C94" s="25">
         <v>44.33</v>
@@ -10369,7 +10360,7 @@
         <v>45</v>
       </c>
       <c r="Z94" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA94" s="24">
         <v>1.0</v>
@@ -10394,14 +10385,14 @@
       </c>
       <c r="AH94" s="21"/>
       <c r="AI94" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ94" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ94" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK94" s="29"/>
       <c r="AL94" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM94" s="6"/>
       <c r="AN94" s="6"/>
@@ -10410,10 +10401,10 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C95" s="25">
         <v>44.2746</v>
@@ -10471,7 +10462,7 @@
         <v>45</v>
       </c>
       <c r="Z95" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA95" s="24">
         <v>1.0</v>
@@ -10480,7 +10471,7 @@
         <v>0.0</v>
       </c>
       <c r="AC95" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD95" s="24">
         <v>6.0</v>
@@ -10498,16 +10489,16 @@
         <v>4.0</v>
       </c>
       <c r="AI95" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ95" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AJ95" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="AK95" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL95" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM95" s="6"/>
       <c r="AN95" s="6"/>
@@ -10516,10 +10507,10 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C96" s="25">
         <v>44.2736</v>
@@ -10577,7 +10568,7 @@
         <v>45</v>
       </c>
       <c r="Z96" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA96" s="24">
         <v>1.0</v>
@@ -10602,14 +10593,14 @@
       </c>
       <c r="AH96" s="21"/>
       <c r="AI96" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ96" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ96" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK96" s="29"/>
       <c r="AL96" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM96" s="6"/>
       <c r="AN96" s="6"/>
@@ -10618,10 +10609,10 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C97" s="25">
         <v>44.26779</v>
@@ -10679,7 +10670,7 @@
         <v>45</v>
       </c>
       <c r="Z97" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA97" s="24">
         <v>1.0</v>
@@ -10704,14 +10695,14 @@
       </c>
       <c r="AH97" s="21"/>
       <c r="AI97" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ97" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ97" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK97" s="29"/>
       <c r="AL97" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM97" s="6"/>
       <c r="AN97" s="6"/>
@@ -10720,10 +10711,10 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C98" s="25">
         <v>44.26643</v>
@@ -10781,7 +10772,7 @@
         <v>45</v>
       </c>
       <c r="Z98" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA98" s="24">
         <v>1.0</v>
@@ -10806,14 +10797,14 @@
       </c>
       <c r="AH98" s="21"/>
       <c r="AI98" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ98" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ98" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK98" s="29"/>
       <c r="AL98" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM98" s="6"/>
       <c r="AN98" s="6"/>
@@ -10822,10 +10813,10 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C99" s="25">
         <v>44.32814</v>
@@ -10883,7 +10874,7 @@
         <v>45</v>
       </c>
       <c r="Z99" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA99" s="24">
         <v>1.0</v>
@@ -10908,14 +10899,14 @@
       </c>
       <c r="AH99" s="21"/>
       <c r="AI99" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ99" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ99" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK99" s="29"/>
       <c r="AL99" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM99" s="6"/>
       <c r="AN99" s="6"/>
@@ -10924,10 +10915,10 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C100" s="25">
         <v>44.26535</v>
@@ -10985,7 +10976,7 @@
         <v>45</v>
       </c>
       <c r="Z100" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA100" s="24">
         <v>1.0</v>
@@ -11010,14 +11001,14 @@
       </c>
       <c r="AH100" s="21"/>
       <c r="AI100" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ100" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ100" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK100" s="29"/>
       <c r="AL100" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM100" s="6"/>
       <c r="AN100" s="6"/>
@@ -11026,10 +11017,10 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C101" s="25">
         <v>44.26537</v>
@@ -11087,7 +11078,7 @@
         <v>45</v>
       </c>
       <c r="Z101" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA101" s="24">
         <v>1.0</v>
@@ -11112,14 +11103,14 @@
       </c>
       <c r="AH101" s="21"/>
       <c r="AI101" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ101" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ101" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="AK101" s="29"/>
       <c r="AL101" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM101" s="6"/>
       <c r="AN101" s="6"/>

</xml_diff>